<commit_message>
Changed word from martini to cocktail to satisfy Reddit audience
</commit_message>
<xml_diff>
--- a/Marketing/Marketing.xlsx
+++ b/Marketing/Marketing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bneal\OneDrive\p\thatspecialflavor\Marketing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da78a188f194f783/p/thatspecialflavor/Marketing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Booze Reviews Channels" sheetId="2" r:id="rId2"/>
+    <sheet name="Cocktail Recipe Channels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Fall n Cherry</t>
   </si>
@@ -181,6 +182,15 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/beerporn</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/wine/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cocktails</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/beer</t>
   </si>
 </sst>
 </file>
@@ -216,8 +226,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,10 +756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,8 +774,38 @@
         <v>51</v>
       </c>
     </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>